<commit_message>
auto border added in bsf v12
</commit_message>
<xml_diff>
--- a/bd customs - june.xlsx
+++ b/bd customs - june.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work for Oriental Express\2024 Months\6.June 24\1. 1th june - 43 ta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work for Oriental Express\Mashines_githubFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -197,7 +197,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="36">
   <si>
     <t>ORIENTAL EXPRESS</t>
   </si>
@@ -301,106 +301,10 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Socks</t>
-  </si>
-  <si>
-    <t>Book</t>
-  </si>
-  <si>
-    <t>Iron Scrap</t>
-  </si>
-  <si>
-    <t>Sewing Machine</t>
-  </si>
-  <si>
     <t>Date: 31.05.24</t>
   </si>
   <si>
     <t>MANIFEST NO: 1/6-24</t>
-  </si>
-  <si>
-    <t>Islam Moja</t>
-  </si>
-  <si>
-    <t>Bongo Moja House</t>
-  </si>
-  <si>
-    <t>Ali Moja Ghor</t>
-  </si>
-  <si>
-    <t>Chowrongi Shoes Materials</t>
-  </si>
-  <si>
-    <t>Malek Printings</t>
-  </si>
-  <si>
-    <t>Sathi Book House</t>
-  </si>
-  <si>
-    <t>Hossain Socks</t>
-  </si>
-  <si>
-    <t>Mona Mia Mojas</t>
-  </si>
-  <si>
-    <t>Mamun Feet Items</t>
-  </si>
-  <si>
-    <t>Imam Moja House</t>
-  </si>
-  <si>
-    <t>Khan Feetwares</t>
-  </si>
-  <si>
-    <t>Hossain Traders</t>
-  </si>
-  <si>
-    <t>Siddique Scrapings</t>
-  </si>
-  <si>
-    <t>Karim Machinaries</t>
-  </si>
-  <si>
-    <t>Sharma Footwares</t>
-  </si>
-  <si>
-    <t>Gupta Majuri's</t>
-  </si>
-  <si>
-    <t>Arith Feet &amp; Foots</t>
-  </si>
-  <si>
-    <t>Onindo Feet Socks</t>
-  </si>
-  <si>
-    <t>Putul Book Corner</t>
-  </si>
-  <si>
-    <t>Das Library's</t>
-  </si>
-  <si>
-    <t>Banu Desi Feets</t>
-  </si>
-  <si>
-    <t>Kiran Feet Fest's</t>
-  </si>
-  <si>
-    <t>Navneet Moja Ghor</t>
-  </si>
-  <si>
-    <t>Kolkata Socks Bazar</t>
-  </si>
-  <si>
-    <t>Himanshi Foot Mantra's</t>
-  </si>
-  <si>
-    <t>Nior Irons</t>
-  </si>
-  <si>
-    <t>Chttarjee Iron Works</t>
-  </si>
-  <si>
-    <t>Nondini's Sewing Center</t>
   </si>
 </sst>
 </file>
@@ -1202,8 +1106,8 @@
   </sheetPr>
   <dimension ref="B1:N105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1312,12 +1216,12 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="54" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F7" s="55"/>
       <c r="G7" s="1"/>
       <c r="H7" s="28" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1447,33 +1351,23 @@
       <c r="B15" s="46">
         <v>1</v>
       </c>
-      <c r="C15" s="47">
-        <v>6065</v>
-      </c>
-      <c r="D15" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="51" t="s">
-        <v>54</v>
-      </c>
+      <c r="C15" s="47"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
       <c r="F15" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G15" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" s="48">
-        <v>8</v>
-      </c>
+      <c r="H15" s="47"/>
+      <c r="I15" s="48"/>
       <c r="J15" s="47">
         <v>1</v>
       </c>
       <c r="K15" s="49">
         <f>INT(I15)*2</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L15" s="27"/>
       <c r="M15" s="43"/>
@@ -1482,33 +1376,23 @@
       <c r="B16" s="46">
         <v>2</v>
       </c>
-      <c r="C16" s="47">
-        <v>6066</v>
-      </c>
-      <c r="D16" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="51" t="s">
-        <v>54</v>
-      </c>
+      <c r="C16" s="47"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
       <c r="F16" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G16" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" s="48">
-        <v>8</v>
-      </c>
+      <c r="H16" s="47"/>
+      <c r="I16" s="48"/>
       <c r="J16" s="47">
         <v>1</v>
       </c>
       <c r="K16" s="49">
         <f>INT(I16)*2</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L16" s="36"/>
       <c r="M16" s="43"/>
@@ -1518,33 +1402,23 @@
       <c r="B17" s="46">
         <v>3</v>
       </c>
-      <c r="C17" s="47">
-        <v>6067</v>
-      </c>
-      <c r="D17" s="51" t="s">
-        <v>40</v>
-      </c>
-      <c r="E17" s="51" t="s">
-        <v>54</v>
-      </c>
+      <c r="C17" s="47"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
       <c r="F17" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G17" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I17" s="48">
-        <v>8</v>
-      </c>
+      <c r="H17" s="47"/>
+      <c r="I17" s="48"/>
       <c r="J17" s="47">
         <v>1</v>
       </c>
       <c r="K17" s="49">
         <f>INT(I17)*2</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L17" s="36"/>
       <c r="M17" s="43"/>
@@ -1553,33 +1427,23 @@
       <c r="B18" s="46">
         <v>4</v>
       </c>
-      <c r="C18" s="47">
-        <v>6068</v>
-      </c>
-      <c r="D18" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="51" t="s">
-        <v>55</v>
-      </c>
+      <c r="C18" s="47"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
       <c r="F18" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G18" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I18" s="48">
-        <v>9</v>
-      </c>
+      <c r="H18" s="47"/>
+      <c r="I18" s="48"/>
       <c r="J18" s="47">
         <v>1</v>
       </c>
       <c r="K18" s="49">
-        <f t="shared" ref="K18:K53" si="0">INT(I18)*2</f>
-        <v>18</v>
+        <f t="shared" ref="K18:K45" si="0">INT(I18)*2</f>
+        <v>0</v>
       </c>
       <c r="L18" s="36"/>
       <c r="M18" s="43"/>
@@ -1588,33 +1452,23 @@
       <c r="B19" s="46">
         <v>5</v>
       </c>
-      <c r="C19" s="47">
-        <v>6069</v>
-      </c>
-      <c r="D19" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="51" t="s">
-        <v>55</v>
-      </c>
+      <c r="C19" s="47"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
       <c r="F19" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G19" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H19" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I19" s="48">
-        <v>9</v>
-      </c>
+      <c r="H19" s="47"/>
+      <c r="I19" s="48"/>
       <c r="J19" s="47">
         <v>1</v>
       </c>
       <c r="K19" s="49">
         <f t="shared" ref="K19:K20" si="1">INT(I19)*2</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="L19" s="36"/>
       <c r="M19" s="43"/>
@@ -1623,33 +1477,23 @@
       <c r="B20" s="46">
         <v>6</v>
       </c>
-      <c r="C20" s="47">
-        <v>6070</v>
-      </c>
-      <c r="D20" s="51" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="51" t="s">
-        <v>55</v>
-      </c>
+      <c r="C20" s="47"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
       <c r="F20" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G20" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H20" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I20" s="48">
-        <v>9</v>
-      </c>
+      <c r="H20" s="47"/>
+      <c r="I20" s="48"/>
       <c r="J20" s="47">
         <v>1</v>
       </c>
       <c r="K20" s="49">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="L20" s="36"/>
       <c r="M20" s="43"/>
@@ -1658,33 +1502,23 @@
       <c r="B21" s="46">
         <v>7</v>
       </c>
-      <c r="C21" s="47">
-        <v>6071</v>
-      </c>
-      <c r="D21" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="E21" s="51" t="s">
-        <v>56</v>
-      </c>
+      <c r="C21" s="47"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
       <c r="F21" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G21" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H21" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I21" s="48">
-        <v>8</v>
-      </c>
+      <c r="H21" s="47"/>
+      <c r="I21" s="48"/>
       <c r="J21" s="47">
         <v>1</v>
       </c>
       <c r="K21" s="49">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L21" s="36"/>
       <c r="M21" s="43"/>
@@ -1693,33 +1527,23 @@
       <c r="B22" s="46">
         <v>8</v>
       </c>
-      <c r="C22" s="47">
-        <v>6072</v>
-      </c>
-      <c r="D22" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" s="51" t="s">
-        <v>56</v>
-      </c>
+      <c r="C22" s="47"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
       <c r="F22" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G22" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H22" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I22" s="48">
-        <v>8</v>
-      </c>
+      <c r="H22" s="47"/>
+      <c r="I22" s="48"/>
       <c r="J22" s="47">
         <v>1</v>
       </c>
       <c r="K22" s="49">
         <f t="shared" ref="K22:K23" si="2">INT(I22)*2</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L22" s="36"/>
       <c r="M22" s="43"/>
@@ -1728,33 +1552,23 @@
       <c r="B23" s="46">
         <v>9</v>
       </c>
-      <c r="C23" s="47">
-        <v>6073</v>
-      </c>
-      <c r="D23" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="51" t="s">
-        <v>56</v>
-      </c>
+      <c r="C23" s="47"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
       <c r="F23" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G23" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H23" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I23" s="48">
-        <v>8</v>
-      </c>
+      <c r="H23" s="47"/>
+      <c r="I23" s="48"/>
       <c r="J23" s="47">
         <v>1</v>
       </c>
       <c r="K23" s="49">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L23" s="36"/>
       <c r="M23" s="43"/>
@@ -1763,33 +1577,23 @@
       <c r="B24" s="46">
         <v>10</v>
       </c>
-      <c r="C24" s="47">
-        <v>6074</v>
-      </c>
-      <c r="D24" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="51" t="s">
-        <v>57</v>
-      </c>
+      <c r="C24" s="47"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="51"/>
       <c r="F24" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G24" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I24" s="48">
-        <v>9</v>
-      </c>
+      <c r="H24" s="47"/>
+      <c r="I24" s="48"/>
       <c r="J24" s="47">
         <v>1</v>
       </c>
       <c r="K24" s="49">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="L24" s="36"/>
       <c r="M24" s="43"/>
@@ -1798,33 +1602,23 @@
       <c r="B25" s="46">
         <v>11</v>
       </c>
-      <c r="C25" s="47">
-        <v>6075</v>
-      </c>
-      <c r="D25" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="51" t="s">
-        <v>57</v>
-      </c>
+      <c r="C25" s="47"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="51"/>
       <c r="F25" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G25" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H25" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I25" s="48">
-        <v>9</v>
-      </c>
+      <c r="H25" s="47"/>
+      <c r="I25" s="48"/>
       <c r="J25" s="47">
         <v>1</v>
       </c>
       <c r="K25" s="49">
         <f t="shared" ref="K25:K26" si="3">INT(I25)*2</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="L25" s="36"/>
       <c r="M25" s="43"/>
@@ -1833,33 +1627,23 @@
       <c r="B26" s="46">
         <v>12</v>
       </c>
-      <c r="C26" s="47">
-        <v>6076</v>
-      </c>
-      <c r="D26" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="51" t="s">
-        <v>57</v>
-      </c>
+      <c r="C26" s="47"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="51"/>
       <c r="F26" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G26" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H26" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I26" s="48">
-        <v>9</v>
-      </c>
+      <c r="H26" s="47"/>
+      <c r="I26" s="48"/>
       <c r="J26" s="47">
         <v>1</v>
       </c>
       <c r="K26" s="49">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="L26" s="36"/>
       <c r="M26" s="43"/>
@@ -1868,33 +1652,23 @@
       <c r="B27" s="46">
         <v>13</v>
       </c>
-      <c r="C27" s="47">
-        <v>6077</v>
-      </c>
-      <c r="D27" s="51" t="s">
-        <v>44</v>
-      </c>
-      <c r="E27" s="51" t="s">
-        <v>58</v>
-      </c>
+      <c r="C27" s="47"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
       <c r="F27" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G27" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H27" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="I27" s="48">
-        <v>9</v>
-      </c>
+      <c r="H27" s="47"/>
+      <c r="I27" s="48"/>
       <c r="J27" s="47">
         <v>1</v>
       </c>
       <c r="K27" s="49">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="L27" s="36"/>
       <c r="M27" s="43"/>
@@ -1903,33 +1677,23 @@
       <c r="B28" s="46">
         <v>14</v>
       </c>
-      <c r="C28" s="47">
-        <v>6078</v>
-      </c>
-      <c r="D28" s="51" t="s">
-        <v>44</v>
-      </c>
-      <c r="E28" s="51" t="s">
-        <v>58</v>
-      </c>
+      <c r="C28" s="47"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
       <c r="F28" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G28" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H28" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="I28" s="48">
-        <v>9</v>
-      </c>
+      <c r="H28" s="47"/>
+      <c r="I28" s="48"/>
       <c r="J28" s="47">
         <v>1</v>
       </c>
       <c r="K28" s="49">
         <f t="shared" ref="K28:K29" si="4">INT(I28)*2</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="L28" s="36"/>
       <c r="M28" s="43"/>
@@ -1938,33 +1702,23 @@
       <c r="B29" s="46">
         <v>15</v>
       </c>
-      <c r="C29" s="47">
-        <v>6079</v>
-      </c>
-      <c r="D29" s="51" t="s">
-        <v>44</v>
-      </c>
-      <c r="E29" s="51" t="s">
-        <v>58</v>
-      </c>
+      <c r="C29" s="47"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
       <c r="F29" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G29" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H29" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="I29" s="48">
-        <v>9</v>
-      </c>
+      <c r="H29" s="47"/>
+      <c r="I29" s="48"/>
       <c r="J29" s="47">
         <v>1</v>
       </c>
       <c r="K29" s="49">
         <f t="shared" si="4"/>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="L29" s="36"/>
       <c r="M29" s="43"/>
@@ -1973,33 +1727,23 @@
       <c r="B30" s="46">
         <v>16</v>
       </c>
-      <c r="C30" s="47">
-        <v>6080</v>
-      </c>
-      <c r="D30" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="E30" s="51" t="s">
-        <v>59</v>
-      </c>
+      <c r="C30" s="47"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
       <c r="F30" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G30" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H30" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="I30" s="48">
-        <v>8</v>
-      </c>
+      <c r="H30" s="47"/>
+      <c r="I30" s="48"/>
       <c r="J30" s="47">
         <v>1</v>
       </c>
       <c r="K30" s="49">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L30" s="36"/>
       <c r="M30" s="43"/>
@@ -2008,33 +1752,23 @@
       <c r="B31" s="46">
         <v>17</v>
       </c>
-      <c r="C31" s="47">
-        <v>6081</v>
-      </c>
-      <c r="D31" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="E31" s="51" t="s">
-        <v>59</v>
-      </c>
+      <c r="C31" s="47"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
       <c r="F31" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G31" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H31" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="I31" s="48">
-        <v>8</v>
-      </c>
+      <c r="H31" s="47"/>
+      <c r="I31" s="48"/>
       <c r="J31" s="47">
         <v>1</v>
       </c>
       <c r="K31" s="49">
         <f t="shared" ref="K31:K32" si="5">INT(I31)*2</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L31" s="36"/>
       <c r="M31" s="43"/>
@@ -2043,33 +1777,23 @@
       <c r="B32" s="46">
         <v>18</v>
       </c>
-      <c r="C32" s="47">
-        <v>6082</v>
-      </c>
-      <c r="D32" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="E32" s="51" t="s">
-        <v>59</v>
-      </c>
+      <c r="C32" s="47"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
       <c r="F32" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G32" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H32" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="I32" s="48">
-        <v>8</v>
-      </c>
+      <c r="H32" s="47"/>
+      <c r="I32" s="48"/>
       <c r="J32" s="47">
         <v>1</v>
       </c>
       <c r="K32" s="49">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L32" s="36"/>
       <c r="M32" s="43"/>
@@ -2078,33 +1802,23 @@
       <c r="B33" s="46">
         <v>19</v>
       </c>
-      <c r="C33" s="47">
-        <v>6083</v>
-      </c>
-      <c r="D33" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" s="51" t="s">
-        <v>60</v>
-      </c>
+      <c r="C33" s="47"/>
+      <c r="D33" s="51"/>
+      <c r="E33" s="51"/>
       <c r="F33" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G33" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H33" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I33" s="48">
-        <v>9</v>
-      </c>
+      <c r="H33" s="47"/>
+      <c r="I33" s="48"/>
       <c r="J33" s="47">
         <v>1</v>
       </c>
       <c r="K33" s="49">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="L33" s="36"/>
       <c r="M33" s="43"/>
@@ -2113,33 +1827,23 @@
       <c r="B34" s="46">
         <v>20</v>
       </c>
-      <c r="C34" s="47">
-        <v>6084</v>
-      </c>
-      <c r="D34" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="E34" s="51" t="s">
-        <v>60</v>
-      </c>
+      <c r="C34" s="47"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
       <c r="F34" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G34" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H34" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I34" s="48">
-        <v>9</v>
-      </c>
+      <c r="H34" s="47"/>
+      <c r="I34" s="48"/>
       <c r="J34" s="47">
         <v>1</v>
       </c>
       <c r="K34" s="49">
         <f t="shared" ref="K34:K35" si="6">INT(I34)*2</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="L34" s="36"/>
       <c r="M34" s="30"/>
@@ -2148,33 +1852,23 @@
       <c r="B35" s="46">
         <v>21</v>
       </c>
-      <c r="C35" s="47">
-        <v>6085</v>
-      </c>
-      <c r="D35" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="E35" s="51" t="s">
-        <v>60</v>
-      </c>
+      <c r="C35" s="47"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="51"/>
       <c r="F35" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G35" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H35" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I35" s="48">
-        <v>9</v>
-      </c>
+      <c r="H35" s="47"/>
+      <c r="I35" s="48"/>
       <c r="J35" s="47">
         <v>1</v>
       </c>
       <c r="K35" s="49">
         <f t="shared" si="6"/>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="L35" s="36"/>
       <c r="M35" s="30"/>
@@ -2183,33 +1877,23 @@
       <c r="B36" s="46">
         <v>22</v>
       </c>
-      <c r="C36" s="47">
-        <v>6086</v>
-      </c>
-      <c r="D36" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="E36" s="51" t="s">
-        <v>61</v>
-      </c>
+      <c r="C36" s="47"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="51"/>
       <c r="F36" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G36" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H36" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I36" s="48">
-        <v>8</v>
-      </c>
+      <c r="H36" s="47"/>
+      <c r="I36" s="48"/>
       <c r="J36" s="47">
         <v>1</v>
       </c>
       <c r="K36" s="49">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L36" s="36"/>
       <c r="M36" s="30"/>
@@ -2218,33 +1902,23 @@
       <c r="B37" s="46">
         <v>23</v>
       </c>
-      <c r="C37" s="47">
-        <v>6087</v>
-      </c>
-      <c r="D37" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="E37" s="51" t="s">
-        <v>61</v>
-      </c>
+      <c r="C37" s="47"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
       <c r="F37" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G37" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H37" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I37" s="48">
-        <v>8</v>
-      </c>
+      <c r="H37" s="47"/>
+      <c r="I37" s="48"/>
       <c r="J37" s="47">
         <v>1</v>
       </c>
       <c r="K37" s="49">
         <f t="shared" ref="K37:K38" si="7">INT(I37)*2</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L37" s="36"/>
       <c r="M37" s="30"/>
@@ -2253,33 +1927,23 @@
       <c r="B38" s="46">
         <v>24</v>
       </c>
-      <c r="C38" s="47">
-        <v>6088</v>
-      </c>
-      <c r="D38" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="E38" s="51" t="s">
-        <v>61</v>
-      </c>
+      <c r="C38" s="47"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="51"/>
       <c r="F38" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G38" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H38" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I38" s="48">
-        <v>8</v>
-      </c>
+      <c r="H38" s="47"/>
+      <c r="I38" s="48"/>
       <c r="J38" s="47">
         <v>1</v>
       </c>
       <c r="K38" s="49">
         <f t="shared" si="7"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L38" s="36"/>
       <c r="M38" s="30"/>
@@ -2288,33 +1952,23 @@
       <c r="B39" s="46">
         <v>25</v>
       </c>
-      <c r="C39" s="47">
-        <v>6089</v>
-      </c>
-      <c r="D39" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="E39" s="51" t="s">
-        <v>62</v>
-      </c>
+      <c r="C39" s="47"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
       <c r="F39" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G39" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H39" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I39" s="48">
-        <v>7</v>
-      </c>
+      <c r="H39" s="47"/>
+      <c r="I39" s="48"/>
       <c r="J39" s="47">
         <v>1</v>
       </c>
       <c r="K39" s="49">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="L39" s="36"/>
       <c r="M39" s="30"/>
@@ -2324,33 +1978,23 @@
       <c r="B40" s="46">
         <v>26</v>
       </c>
-      <c r="C40" s="47">
-        <v>6090</v>
-      </c>
-      <c r="D40" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="E40" s="51" t="s">
-        <v>62</v>
-      </c>
+      <c r="C40" s="47"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="51"/>
       <c r="F40" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G40" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H40" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I40" s="48">
-        <v>7</v>
-      </c>
+      <c r="H40" s="47"/>
+      <c r="I40" s="48"/>
       <c r="J40" s="47">
         <v>1</v>
       </c>
       <c r="K40" s="49">
         <f t="shared" ref="K40:K41" si="8">INT(I40)*2</f>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="L40" s="36"/>
       <c r="M40" s="30"/>
@@ -2360,33 +2004,23 @@
       <c r="B41" s="46">
         <v>27</v>
       </c>
-      <c r="C41" s="47">
-        <v>6091</v>
-      </c>
-      <c r="D41" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="E41" s="51" t="s">
-        <v>62</v>
-      </c>
+      <c r="C41" s="47"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="51"/>
       <c r="F41" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G41" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H41" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I41" s="48">
-        <v>7</v>
-      </c>
+      <c r="H41" s="47"/>
+      <c r="I41" s="48"/>
       <c r="J41" s="47">
         <v>1</v>
       </c>
       <c r="K41" s="49">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="L41" s="36"/>
       <c r="M41" s="30"/>
@@ -2395,33 +2029,23 @@
       <c r="B42" s="46">
         <v>28</v>
       </c>
-      <c r="C42" s="47">
-        <v>6092</v>
-      </c>
-      <c r="D42" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="E42" s="51" t="s">
-        <v>63</v>
-      </c>
+      <c r="C42" s="47"/>
+      <c r="D42" s="51"/>
+      <c r="E42" s="51"/>
       <c r="F42" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G42" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H42" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I42" s="48">
-        <v>9</v>
-      </c>
+      <c r="H42" s="47"/>
+      <c r="I42" s="48"/>
       <c r="J42" s="47">
         <v>1</v>
       </c>
       <c r="K42" s="49">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="L42" s="36"/>
       <c r="M42" s="30"/>
@@ -2430,33 +2054,23 @@
       <c r="B43" s="46">
         <v>29</v>
       </c>
-      <c r="C43" s="47">
-        <v>6093</v>
-      </c>
-      <c r="D43" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="E43" s="51" t="s">
-        <v>63</v>
-      </c>
+      <c r="C43" s="47"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="51"/>
       <c r="F43" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G43" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H43" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I43" s="48">
-        <v>9</v>
-      </c>
+      <c r="H43" s="47"/>
+      <c r="I43" s="48"/>
       <c r="J43" s="47">
         <v>1</v>
       </c>
       <c r="K43" s="49">
         <f t="shared" ref="K43:K44" si="9">INT(I43)*2</f>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="L43" s="36"/>
       <c r="M43" s="30"/>
@@ -2465,33 +2079,23 @@
       <c r="B44" s="46">
         <v>30</v>
       </c>
-      <c r="C44" s="47">
-        <v>6094</v>
-      </c>
-      <c r="D44" s="51" t="s">
-        <v>49</v>
-      </c>
-      <c r="E44" s="51" t="s">
-        <v>63</v>
-      </c>
+      <c r="C44" s="47"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="51"/>
       <c r="F44" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G44" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H44" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I44" s="48">
-        <v>9</v>
-      </c>
+      <c r="H44" s="47"/>
+      <c r="I44" s="48"/>
       <c r="J44" s="47">
         <v>1</v>
       </c>
       <c r="K44" s="49">
         <f t="shared" si="9"/>
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="L44" s="36"/>
       <c r="M44" s="30"/>
@@ -2500,33 +2104,23 @@
       <c r="B45" s="46">
         <v>31</v>
       </c>
-      <c r="C45" s="47">
-        <v>6095</v>
-      </c>
-      <c r="D45" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="E45" s="51" t="s">
-        <v>64</v>
-      </c>
+      <c r="C45" s="47"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="51"/>
       <c r="F45" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G45" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H45" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I45" s="50">
-        <v>8</v>
-      </c>
+      <c r="H45" s="47"/>
+      <c r="I45" s="50"/>
       <c r="J45" s="47">
         <v>1</v>
       </c>
       <c r="K45" s="49">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L45" s="36"/>
       <c r="M45" s="30"/>
@@ -2535,33 +2129,23 @@
       <c r="B46" s="46">
         <v>32</v>
       </c>
-      <c r="C46" s="47">
-        <v>6096</v>
-      </c>
-      <c r="D46" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="E46" s="51" t="s">
-        <v>64</v>
-      </c>
+      <c r="C46" s="47"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="51"/>
       <c r="F46" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G46" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H46" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I46" s="50">
-        <v>8</v>
-      </c>
+      <c r="H46" s="47"/>
+      <c r="I46" s="50"/>
       <c r="J46" s="47">
         <v>1</v>
       </c>
       <c r="K46" s="49">
         <f t="shared" ref="K46:K47" si="10">INT(I46)*2</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L46" s="36"/>
     </row>
@@ -2569,330 +2153,230 @@
       <c r="B47" s="46">
         <v>33</v>
       </c>
-      <c r="C47" s="47">
-        <v>6097</v>
-      </c>
-      <c r="D47" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="E47" s="51" t="s">
-        <v>64</v>
-      </c>
+      <c r="C47" s="47"/>
+      <c r="D47" s="51"/>
+      <c r="E47" s="51"/>
       <c r="F47" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G47" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H47" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="I47" s="50">
-        <v>8</v>
-      </c>
+      <c r="H47" s="47"/>
+      <c r="I47" s="50"/>
       <c r="J47" s="47">
         <v>1</v>
       </c>
       <c r="K47" s="49">
         <f t="shared" si="10"/>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="2:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B48" s="46">
         <v>34</v>
       </c>
-      <c r="C48" s="47">
-        <v>6098</v>
-      </c>
-      <c r="D48" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="E48" s="51" t="s">
-        <v>65</v>
-      </c>
+      <c r="C48" s="47"/>
+      <c r="D48" s="51"/>
+      <c r="E48" s="51"/>
       <c r="F48" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G48" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H48" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="I48" s="48">
-        <v>8</v>
-      </c>
+      <c r="H48" s="47"/>
+      <c r="I48" s="48"/>
       <c r="J48" s="47">
         <v>1</v>
       </c>
       <c r="K48" s="49">
-        <f t="shared" ref="K48:K49" si="11">INT(I48)*2</f>
-        <v>16</v>
+        <f t="shared" ref="K48" si="11">INT(I48)*2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B49" s="46">
         <v>35</v>
       </c>
-      <c r="C49" s="47">
-        <v>6099</v>
-      </c>
-      <c r="D49" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="E49" s="51" t="s">
-        <v>65</v>
-      </c>
+      <c r="C49" s="47"/>
+      <c r="D49" s="51"/>
+      <c r="E49" s="51"/>
       <c r="F49" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G49" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H49" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="I49" s="48">
-        <v>8</v>
-      </c>
+      <c r="H49" s="47"/>
+      <c r="I49" s="48"/>
       <c r="J49" s="47">
         <v>1</v>
       </c>
       <c r="K49" s="49">
         <f t="shared" ref="K49:K50" si="12">INT(I49)*2</f>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B50" s="46">
         <v>36</v>
       </c>
-      <c r="C50" s="47">
-        <v>6100</v>
-      </c>
-      <c r="D50" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="E50" s="51" t="s">
-        <v>65</v>
-      </c>
+      <c r="C50" s="47"/>
+      <c r="D50" s="51"/>
+      <c r="E50" s="51"/>
       <c r="F50" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G50" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H50" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="I50" s="48">
-        <v>8</v>
-      </c>
+      <c r="H50" s="47"/>
+      <c r="I50" s="48"/>
       <c r="J50" s="47">
         <v>1</v>
       </c>
       <c r="K50" s="49">
         <f t="shared" si="12"/>
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B51" s="46">
         <v>37</v>
       </c>
-      <c r="C51" s="47">
-        <v>6101</v>
-      </c>
-      <c r="D51" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="E51" s="51" t="s">
-        <v>66</v>
-      </c>
+      <c r="C51" s="47"/>
+      <c r="D51" s="51"/>
+      <c r="E51" s="51"/>
       <c r="F51" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G51" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H51" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="I51" s="48">
-        <v>9</v>
-      </c>
+      <c r="H51" s="47"/>
+      <c r="I51" s="48"/>
       <c r="J51" s="47">
         <v>1</v>
       </c>
       <c r="K51" s="49">
-        <f t="shared" ref="K51:K52" si="13">INT(I51)*2</f>
-        <v>18</v>
+        <f t="shared" ref="K51" si="13">INT(I51)*2</f>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B52" s="46">
         <v>38</v>
       </c>
-      <c r="C52" s="47">
-        <v>6102</v>
-      </c>
-      <c r="D52" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="E52" s="51" t="s">
-        <v>66</v>
-      </c>
+      <c r="C52" s="47"/>
+      <c r="D52" s="51"/>
+      <c r="E52" s="51"/>
       <c r="F52" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G52" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H52" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="I52" s="48">
-        <v>9</v>
-      </c>
+      <c r="H52" s="47"/>
+      <c r="I52" s="48"/>
       <c r="J52" s="47">
         <v>1</v>
       </c>
       <c r="K52" s="49">
         <f t="shared" ref="K52:K53" si="14">INT(I52)*2</f>
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B53" s="46">
         <v>39</v>
       </c>
-      <c r="C53" s="47">
-        <v>6103</v>
-      </c>
-      <c r="D53" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="E53" s="51" t="s">
-        <v>66</v>
-      </c>
+      <c r="C53" s="47"/>
+      <c r="D53" s="51"/>
+      <c r="E53" s="51"/>
       <c r="F53" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G53" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H53" s="47" t="s">
-        <v>36</v>
-      </c>
-      <c r="I53" s="48">
-        <v>9</v>
-      </c>
+      <c r="H53" s="47"/>
+      <c r="I53" s="48"/>
       <c r="J53" s="47">
         <v>1</v>
       </c>
       <c r="K53" s="49">
         <f t="shared" si="14"/>
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B54" s="46">
         <v>40</v>
       </c>
-      <c r="C54" s="47">
-        <v>6104</v>
-      </c>
-      <c r="D54" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="E54" s="51" t="s">
-        <v>67</v>
-      </c>
+      <c r="C54" s="47"/>
+      <c r="D54" s="51"/>
+      <c r="E54" s="51"/>
       <c r="F54" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G54" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H54" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="I54" s="50">
-        <v>7</v>
-      </c>
+      <c r="H54" s="47"/>
+      <c r="I54" s="50"/>
       <c r="J54" s="47">
         <v>1</v>
       </c>
       <c r="K54" s="49">
         <f>INT(I54)*3</f>
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B55" s="46">
         <v>41</v>
       </c>
-      <c r="C55" s="47">
-        <v>6105</v>
-      </c>
-      <c r="D55" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="E55" s="51" t="s">
-        <v>67</v>
-      </c>
+      <c r="C55" s="47"/>
+      <c r="D55" s="51"/>
+      <c r="E55" s="51"/>
       <c r="F55" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G55" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H55" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="I55" s="50">
-        <v>7</v>
-      </c>
+      <c r="H55" s="47"/>
+      <c r="I55" s="50"/>
       <c r="J55" s="47">
         <v>1</v>
       </c>
       <c r="K55" s="49">
         <f>INT(I55)*3</f>
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B56" s="46">
         <v>42</v>
       </c>
-      <c r="C56" s="47">
-        <v>6106</v>
-      </c>
-      <c r="D56" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="E56" s="51" t="s">
-        <v>67</v>
-      </c>
+      <c r="C56" s="47"/>
+      <c r="D56" s="51"/>
+      <c r="E56" s="51"/>
       <c r="F56" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G56" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H56" s="47" t="s">
-        <v>37</v>
-      </c>
-      <c r="I56" s="50">
-        <v>7</v>
-      </c>
+      <c r="H56" s="47"/>
+      <c r="I56" s="50"/>
       <c r="J56" s="47">
         <v>1</v>
       </c>
       <c r="K56" s="49">
         <f>INT(I56)*3</f>
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -2907,14 +2391,14 @@
       </c>
       <c r="I57" s="32">
         <f>SUM(I15:I56)</f>
-        <v>348</v>
+        <v>0</v>
       </c>
       <c r="J57" s="31" t="s">
         <v>33</v>
       </c>
       <c r="K57" s="33">
         <f>SUM(K15:K56)</f>
-        <v>717</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>